<commit_message>
Added and assigned footprints, generated netlist
</commit_message>
<xml_diff>
--- a/icarus_bom.xlsx
+++ b/icarus_bom.xlsx
@@ -690,8 +690,8 @@
   </sheetPr>
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E42" activeCellId="0" sqref="E42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Updated BOM, updated layout to fix design rules
</commit_message>
<xml_diff>
--- a/icarus_bom.xlsx
+++ b/icarus_bom.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="189">
   <si>
     <t xml:space="preserve">Item #</t>
   </si>
@@ -49,9 +49,6 @@
     <t xml:space="preserve">Your Instructions/Notes</t>
   </si>
   <si>
-    <t xml:space="preserve"> Value</t>
-  </si>
-  <si>
     <t xml:space="preserve">Digi-Key/Mouser Link</t>
   </si>
   <si>
@@ -64,13 +61,34 @@
     <t xml:space="preserve">C0402C103K5RECAUTO</t>
   </si>
   <si>
+    <t xml:space="preserve">CAP CER 10NF 50V 0402</t>
+  </si>
+  <si>
     <t xml:space="preserve">0402</t>
   </si>
   <si>
     <t xml:space="preserve">SMD</t>
   </si>
   <si>
-    <t xml:space="preserve">10nF</t>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">NOTE:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> For all items I have included a link to Digi-Key or Mouser. It does not matter if the items are purchased from these sites or not, I included them as reference in case any of the manufacturer, manufacturer part numbers, or footprints are unclear.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.com/en/products/detail/kemet/C0402C103K5RECAUTO/8646477</t>
@@ -85,7 +103,7 @@
     <t xml:space="preserve">GMC04X7R103K6R3NT</t>
   </si>
   <si>
-    <t xml:space="preserve">0.01uF</t>
+    <t xml:space="preserve">CAP CER  0.01UF 6.3V 0402</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.com/en/products/detail/cal-chip-electronics-inc/GMC04X7R103K6R3NT/13908424</t>
@@ -100,7 +118,7 @@
     <t xml:space="preserve">GRJ155R60J106ME11D</t>
   </si>
   <si>
-    <t xml:space="preserve">10uF</t>
+    <t xml:space="preserve">CAP CER  10UF 6.3V 0402</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.com/en/products/detail/murata-electronics/GRJ155R60J106ME11D/5877374</t>
@@ -115,12 +133,12 @@
     <t xml:space="preserve">C2012X7S2A105K125AB</t>
   </si>
   <si>
+    <t xml:space="preserve">CAP CER  1UF 100V 0805</t>
+  </si>
+  <si>
     <t xml:space="preserve">0805</t>
   </si>
   <si>
-    <t xml:space="preserve">1uF, 100V</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.digikey.com/en/products/detail/tdk-corporation/C2012X7S2A105K125AB/2116321</t>
   </si>
   <si>
@@ -130,7 +148,7 @@
     <t xml:space="preserve">GRM155R62A104KE14D</t>
   </si>
   <si>
-    <t xml:space="preserve">0.1uF, 100V</t>
+    <t xml:space="preserve">CAP CER  0.1UF 100V 0402</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.com/en/products/detail/murata-electronics/GRM155R62A104KE14D/5027543</t>
@@ -145,7 +163,7 @@
     <t xml:space="preserve">CC0402KRX5R5BB105</t>
   </si>
   <si>
-    <t xml:space="preserve">1uF</t>
+    <t xml:space="preserve">CAP CER  1UF 6.3V 0402</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.com/en/products/detail/yageo/CC0402KRX5R5BB105/2833603</t>
@@ -157,43 +175,46 @@
     <t xml:space="preserve">GMC04X5R104K10NT</t>
   </si>
   <si>
-    <t xml:space="preserve">0.1uF</t>
+    <t xml:space="preserve">CAP CER  0.1UF 10V 0402</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.com/en/products/detail/cal-chip-electronics-inc/GMC04X5R104K10NT/13908671</t>
   </si>
   <si>
+    <t xml:space="preserve">CR1 CR2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vishay General Semiconductor - Diodes Division</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMBJ51CA-E3/52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIODE 82.4V 600W DO-214AA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DO-214AA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/en/products/detail/vishay-semiconductor-diodes-division/smbj51ca-e3-52/1119303</t>
+  </si>
+  <si>
     <t xml:space="preserve">D1 </t>
   </si>
   <si>
     <t xml:space="preserve">ON Semiconductor</t>
   </si>
   <si>
+    <t xml:space="preserve">DIODE 30V 200MA SOD-523F</t>
+  </si>
+  <si>
     <t xml:space="preserve">SOD-523F</t>
   </si>
   <si>
-    <t xml:space="preserve">RB520S30</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.digikey.com/en/products/detail/on-semiconductor/rb520s30/1955134</t>
   </si>
   <si>
-    <t xml:space="preserve">D2 D3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vishay General Semiconductor - Diodes Division</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMBJ51CA-E3/52</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DO-214AA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/vishay-semiconductor-diodes-division/smbj51ca-e3-52/1119303</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D5 D4 </t>
+    <t xml:space="preserve">D3 D2 </t>
   </si>
   <si>
     <t xml:space="preserve">Kingbright</t>
@@ -202,16 +223,16 @@
     <t xml:space="preserve">APT1608CGCK</t>
   </si>
   <si>
+    <t xml:space="preserve">LED 0603 GREEN</t>
+  </si>
+  <si>
     <t xml:space="preserve">0603</t>
   </si>
   <si>
-    <t xml:space="preserve">Green</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.digikey.com/en/products/detail/kingbright/APT1608CGCK/1747514</t>
   </si>
   <si>
-    <t xml:space="preserve">D6 D7 D8 D9 </t>
+    <t xml:space="preserve">D4 D5 D6 D7 </t>
   </si>
   <si>
     <t xml:space="preserve">Rohm Semiconductor</t>
@@ -220,22 +241,25 @@
     <t xml:space="preserve">SMLE13BC8TT86</t>
   </si>
   <si>
-    <t xml:space="preserve">Blue</t>
+    <t xml:space="preserve">LED 0603 BLUE</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.com/en/products/detail/rohm-semiconductor/SMLE13BC8TT86/5053771</t>
   </si>
   <si>
-    <t xml:space="preserve">J1 J2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAN Bus</t>
-  </si>
-  <si>
     <t xml:space="preserve">J4 </t>
   </si>
   <si>
-    <t xml:space="preserve">USB_B_Micro</t>
+    <t xml:space="preserve">Molex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN MICRO USB B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMD/Thru-hole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/en/products/detail/molex/0475890001/1832253</t>
   </si>
   <si>
     <t xml:space="preserve">L1 </t>
@@ -247,16 +271,16 @@
     <t xml:space="preserve">CBC3225T330KR</t>
   </si>
   <si>
+    <t xml:space="preserve">INDUCTOR 33UH 533MOHM 1210</t>
+  </si>
+  <si>
     <t xml:space="preserve">1210</t>
   </si>
   <si>
-    <t xml:space="preserve">33uH</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.digikey.com/en/products/detail/taiyo-yuden/CBC3225T330KR/2763320</t>
   </si>
   <si>
-    <t xml:space="preserve">M1 M2 M4 </t>
+    <t xml:space="preserve">MOSFET1 MOSFET3 MOSFET5 </t>
   </si>
   <si>
     <t xml:space="preserve">Nexperia USA Inc.</t>
@@ -265,19 +289,40 @@
     <t xml:space="preserve">PSMN4R8-100BSEJ</t>
   </si>
   <si>
+    <t xml:space="preserve">N-CHANNEL MOSFET 100V 120A D2PAK</t>
+  </si>
+  <si>
     <t xml:space="preserve">D2PAK</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.com/en/products/detail/nexperia-usa-inc/PSMN4R8-100BSEJ/4020506?s=N4IgTCBcDaIAoGUCyA5ALAJQBwFoCMADAQEIICiAUiALoC%2BQA</t>
   </si>
   <si>
-    <t xml:space="preserve">M3 </t>
+    <t xml:space="preserve">MOSFET2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diodes Incorporated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZXMP10A13FTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P-CHANNEL MOSFET 100V 600MA SOT-23-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOT-23-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/en/products/detail/diodes-incorporated/zxmp10a13fta/560644</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOSFET4 </t>
   </si>
   <si>
     <t xml:space="preserve">BSS123</t>
   </si>
   <si>
-    <t xml:space="preserve">SOT-23-3</t>
+    <t xml:space="preserve">N-CHANNEL MOSFET 100V 170MA SOT-23-3</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.com/en/products/detail/on-semiconductor/BSS123/244348</t>
@@ -292,147 +337,144 @@
     <t xml:space="preserve">CSNL2512FTL500</t>
   </si>
   <si>
+    <t xml:space="preserve">RESISTOR 500UOHM 1% 2W 2512</t>
+  </si>
+  <si>
     <t xml:space="preserve">2512</t>
   </si>
   <si>
-    <t xml:space="preserve">0.5m</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.digikey.com/en/products/detail/stackpole-electronics-inc/CSNL2512FTL500/1788105</t>
   </si>
   <si>
-    <t xml:space="preserve">R10 </t>
+    <t xml:space="preserve">R14 R2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0402FR-0747KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESITOR 47K OHM 1% 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/en/products/detail/yageo/RC0402FR-0747KL/726616</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R15 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panasonic Electronic Components</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-2GEJ474X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESISTOR 470K OHM 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/en/products/detail/panasonic-electronic-components/ERJ-2GEJ474X/147018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R16 R17 R18 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venkel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR0402-16W-6801FT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESISTOR 6.8 KOHM 1% 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/en/products/detail/venkel/CR0402-16W-6801FT/12329730</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R20 R19 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0603FR-073ML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESISTOR 3M OHM 0603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/en/products/detail/yageo/RC0603FR-073ML/5918344?s=N4IgTCBcDaIEoGEAMA2JBmAYnAtEg7OgLIAyIAugL5A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R22 R21 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0402FR-07200KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESISTOR 200K OHM 1% 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/en/products/detail/yageo/RC0402FR-07200KL/726558</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R3 R8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0402FR-07100KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESISTOR 100K OHM 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/en/products/detail/yageo/RC0402FR-07100KL/726526</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R5 R10 R4 R11 R12 R13 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR0402-16W-221JT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESISTOR 220 OHM 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/en/products/detail/venkel/CR0402-16W-221JT/12329552</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0402JR-0710RL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESISTOR 10 OHM 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/en/products/detail/yageo/RC0402JR-0710RL/726417</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KOA Speer Electronics, Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RK73H1ETTP4993F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESISTOR 499K OHM 1% 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/en/products/detail/koa-speer-electronics-inc/RK73H1ETTP4993F/9844110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R9 </t>
   </si>
   <si>
     <t xml:space="preserve">RC0402FR-07140KL</t>
   </si>
   <si>
-    <t xml:space="preserve">140k, 1%</t>
+    <t xml:space="preserve">RESISTOR 140K OHM 1% 0402</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.com/en/products/detail/yageo/RC0402FR-07140KL/5280838</t>
   </si>
   <si>
-    <t xml:space="preserve">R15 R3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0402FR-0747KL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47k, 1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/yageo/RC0402FR-0747KL/726616</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R16 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Venkel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CR0402-16W-6801FT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.8k, 1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/venkel/CR0402-16W-6801FT/12329730</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R17 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">R_Small</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R19 R18 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0603FR-073ML</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3M, 1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/yageo/RC0603FR-073ML/5918344?s=N4IgTCBcDaIEoGEAMA2JBmAYnAtEg7OgLIAyIAugL5A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Panasonic Electronic Components</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERJ-2GEJ474X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">470k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/panasonic-electronic-components/ERJ-2GEJ474X/147018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R21 R20 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0402FR-07200KL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">200k, 1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/yageo/RC0402FR-07200KL/726558</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Samsung Electro-Mechanics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC1005F103CS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/samsung-electro-mechanics/RC1005F103CS/3903439</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R5 R9 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0402FR-07100KL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/yageo/RC0402FR-07100KL/726526</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R7 R11 R6 R12 R13 R14 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0402FR-0722RL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/yageo/RC0402FR-0722RL/726562</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R8 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">KOA Speer Electronics, Inc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RK73H1ETTP4993F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">499k, 1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/koa-speer-electronics-inc/RK73H1ETTP4993F/9844110</t>
-  </si>
-  <si>
     <t xml:space="preserve">U1 </t>
   </si>
   <si>
@@ -442,60 +484,63 @@
     <t xml:space="preserve">MAX15062AATA+T</t>
   </si>
   <si>
+    <t xml:space="preserve">IC VOLTAGE REGULATOR 3.3V 300MA 8-WFDFN</t>
+  </si>
+  <si>
     <t xml:space="preserve">8-WFDFN</t>
   </si>
   <si>
-    <t xml:space="preserve">MAX15062A</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.digikey.com/en/products/detail/maxim-integrated/MAX15062AATA-T/2591307?s=N4IgTCBcDaILIEEAaBGArABgGxgSAugL5A</t>
   </si>
   <si>
+    <t xml:space="preserve">U13 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analog Devices Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LT1787HVIMS8#PBF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC CURRENSE SENSE AMPLIFIER 8-MSOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8-MSOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.com/ProductDetail/Analog-Devices/LT1787HVIMS8PBF?qs=%2Fha2pyFadujK7yAATxqvcekSDFITlKcvQA8DNiibuHwxpwWvAriAAg%3D%3D</t>
+  </si>
+  <si>
     <t xml:space="preserve">U14 </t>
   </si>
   <si>
-    <t xml:space="preserve">Analog Devices Inc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LT1787HVIMS8#PBF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8-MSOP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LT1787HVIMS8PBF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.mouser.com/ProductDetail/Analog-Devices/LT1787HVIMS8PBF?qs=%2Fha2pyFadujK7yAATxqvcekSDFITlKcvQA8DNiibuHwxpwWvAriAAg%3D%3D</t>
+    <t xml:space="preserve">STMicroelectronics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USBLC6-2SC6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIODE 17V 5A SOT-23-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOT-23-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/en/products/detail/stmicroelectronics/USBLC6-2SC6/1040559</t>
   </si>
   <si>
     <t xml:space="preserve">U15 </t>
   </si>
   <si>
-    <t xml:space="preserve">STMicroelectronics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USBLC6-2SC6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOT-23-6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/stmicroelectronics/USBLC6-2SC6/1040559</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U16 </t>
-  </si>
-  <si>
     <t xml:space="preserve">STLM20DD9F</t>
   </si>
   <si>
+    <t xml:space="preserve">IC TEMPERATURE SENSOR 4-UDFN</t>
+  </si>
+  <si>
     <t xml:space="preserve">4-UDFN</t>
   </si>
   <si>
-    <t xml:space="preserve">STLM20DD9FUDFN-4L_STM-L</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.digikey.com/en/products/detail/stmicroelectronics/STLM20DD9F/1506426?s=N4IgTCBcDaIM4BcA2BbMAGAJpkBdAvkA</t>
   </si>
   <si>
@@ -505,6 +550,9 @@
     <t xml:space="preserve">STM32G474CEU6</t>
   </si>
   <si>
+    <t xml:space="preserve">IC STM32G474CEU6 48-UFQFPN</t>
+  </si>
+  <si>
     <t xml:space="preserve">48-UFQFPN</t>
   </si>
   <si>
@@ -520,52 +568,43 @@
     <t xml:space="preserve">TCAN334GDR</t>
   </si>
   <si>
+    <t xml:space="preserve">IC CAN BUS DRIVER 8-SOIC</t>
+  </si>
+  <si>
     <t xml:space="preserve">8-SOIC</t>
   </si>
   <si>
-    <t xml:space="preserve">TCAN334G</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.digikey.com/en/products/detail/texas-instruments/TCAN334GDR/5957539</t>
   </si>
   <si>
-    <t xml:space="preserve">U4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diodes Incorporated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZXMP10A13FTA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/diodes-incorporated/zxmp10a13fta/560644</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U6 </t>
+    <t xml:space="preserve">U5 </t>
   </si>
   <si>
     <t xml:space="preserve">FSV10150V</t>
   </si>
   <si>
+    <t xml:space="preserve">DIODE 150V 10A TO-277-3</t>
+  </si>
+  <si>
     <t xml:space="preserve">TO-277-3</t>
   </si>
   <si>
-    <t xml:space="preserve">FSV10150VTO277-3L_ONS-L</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.digikey.com/en/products/detail/on-semiconductor/fsv10150v/5306658</t>
   </si>
   <si>
-    <t xml:space="preserve">U9 </t>
+    <t xml:space="preserve">U8 </t>
   </si>
   <si>
     <t xml:space="preserve">TPS2490DGSR</t>
   </si>
   <si>
+    <t xml:space="preserve">IC HOT SWAP CONTROLLER 10-VSSOP</t>
+  </si>
+  <si>
     <t xml:space="preserve">10-VSSOP</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/texas-instruments/TPS2490DGSR/1671190</t>
+    <t xml:space="preserve">https://www.mouser.com/ProductDetail/Texas-Instruments/TPS2490DGSR?qs=zwk82MlA57aRYVQqxqtqHA%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -581,6 +620,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -602,6 +642,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -646,7 +687,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -671,6 +712,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -688,22 +733,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
+      <selection pane="topLeft" activeCell="F42" activeCellId="0" sqref="F42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="26.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="26.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="41.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="44.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="26.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="38.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="43.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="38.39"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -737,24 +784,24 @@
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -763,10 +810,10 @@
       <c r="H2" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="I2" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="J2" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="0" t="s">
         <v>17</v>
       </c>
     </row>
@@ -786,6 +833,9 @@
       <c r="E3" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="F3" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
@@ -793,9 +843,6 @@
         <v>15</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="0" t="s">
         <v>22</v>
       </c>
     </row>
@@ -815,6 +862,9 @@
       <c r="E4" s="0" t="s">
         <v>25</v>
       </c>
+      <c r="F4" s="0" t="s">
+        <v>26</v>
+      </c>
       <c r="G4" s="1" t="s">
         <v>14</v>
       </c>
@@ -822,9 +872,6 @@
         <v>15</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" s="0" t="s">
         <v>27</v>
       </c>
     </row>
@@ -844,16 +891,16 @@
       <c r="E5" s="0" t="s">
         <v>30</v>
       </c>
+      <c r="F5" s="0" t="s">
+        <v>31</v>
+      </c>
       <c r="G5" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>15</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="K5" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -873,6 +920,9 @@
       <c r="E6" s="0" t="s">
         <v>35</v>
       </c>
+      <c r="F6" s="0" t="s">
+        <v>36</v>
+      </c>
       <c r="G6" s="1" t="s">
         <v>14</v>
       </c>
@@ -880,9 +930,6 @@
         <v>15</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="K6" s="0" t="s">
         <v>37</v>
       </c>
     </row>
@@ -902,6 +949,9 @@
       <c r="E7" s="0" t="s">
         <v>40</v>
       </c>
+      <c r="F7" s="0" t="s">
+        <v>41</v>
+      </c>
       <c r="G7" s="1" t="s">
         <v>14</v>
       </c>
@@ -909,9 +959,6 @@
         <v>15</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="K7" s="0" t="s">
         <v>42</v>
       </c>
     </row>
@@ -931,6 +978,9 @@
       <c r="E8" s="0" t="s">
         <v>44</v>
       </c>
+      <c r="F8" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="G8" s="1" t="s">
         <v>14</v>
       </c>
@@ -938,9 +988,6 @@
         <v>15</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="K8" s="0" t="s">
         <v>46</v>
       </c>
     </row>
@@ -952,25 +999,25 @@
         <v>47</v>
       </c>
       <c r="C9" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>48</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>50</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H9" s="0" t="s">
         <v>15</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="K9" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -978,28 +1025,28 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C10" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>54</v>
       </c>
+      <c r="F10" s="0" t="s">
+        <v>55</v>
+      </c>
       <c r="G10" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H10" s="0" t="s">
         <v>15</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="K10" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1007,28 +1054,28 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C11" s="5" t="n">
         <v>2</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>61</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H11" s="0" t="s">
         <v>15</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="K11" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1036,28 +1083,28 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C12" s="5" t="n">
         <v>4</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>67</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H12" s="0" t="s">
         <v>15</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="K12" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1065,16 +1112,25 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C13" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J13" s="0" t="s">
-        <v>69</v>
+        <v>1</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" s="4" t="n">
+        <v>475890001</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1082,16 +1138,28 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C14" s="5" t="n">
         <v>1</v>
       </c>
+      <c r="D14" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="H14" s="0" t="s">
         <v>15</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1099,28 +1167,28 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="C15" s="5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>74</v>
+        <v>82</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>83</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="H15" s="0" t="s">
         <v>15</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="K15" s="0" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1128,28 +1196,28 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="C16" s="5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>80</v>
+        <v>88</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>89</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="H16" s="0" t="s">
         <v>15</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="K16" s="0" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1157,28 +1225,28 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="C17" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>84</v>
+        <v>93</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>94</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="H17" s="0" t="s">
         <v>15</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="K17" s="0" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1186,28 +1254,28 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="C18" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>89</v>
+        <v>98</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>99</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="H18" s="0" t="s">
         <v>15</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="K18" s="0" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1215,16 +1283,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="C19" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>39</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>94</v>
+        <v>103</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>104</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>14</v>
@@ -1233,10 +1304,7 @@
         <v>15</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="K19" s="0" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1244,16 +1312,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="C20" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>39</v>
+        <v>107</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>98</v>
+        <v>108</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>109</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>14</v>
@@ -1262,10 +1333,7 @@
         <v>15</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="K20" s="0" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1273,16 +1341,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="C21" s="5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>103</v>
+        <v>113</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>114</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>14</v>
@@ -1291,10 +1362,7 @@
         <v>15</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="K21" s="0" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1302,16 +1370,28 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="C22" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="H22" s="0" t="s">
         <v>15</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1319,7 +1399,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="C23" s="5" t="n">
         <v>2</v>
@@ -1328,19 +1408,19 @@
         <v>39</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>109</v>
+        <v>121</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>122</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="H23" s="0" t="s">
         <v>15</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="K23" s="0" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1348,16 +1428,19 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C24" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>114</v>
+        <v>125</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>14</v>
@@ -1366,10 +1449,7 @@
         <v>15</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="K24" s="0" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1377,16 +1457,19 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C25" s="5" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>39</v>
+        <v>112</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>118</v>
+        <v>129</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>130</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>14</v>
@@ -1395,10 +1478,7 @@
         <v>15</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="K25" s="0" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1406,16 +1486,19 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="C26" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>122</v>
+        <v>39</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>123</v>
+        <v>133</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>134</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>14</v>
@@ -1423,11 +1506,8 @@
       <c r="H26" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="J26" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="K26" s="0" t="s">
-        <v>124</v>
+      <c r="J26" s="0" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1435,16 +1515,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="C27" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>39</v>
+        <v>137</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>126</v>
+        <v>138</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>139</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>14</v>
@@ -1452,11 +1535,8 @@
       <c r="H27" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="J27" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="K27" s="0" t="s">
-        <v>128</v>
+      <c r="J27" s="0" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1464,16 +1544,19 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="C28" s="5" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>39</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>130</v>
+        <v>142</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>143</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>14</v>
@@ -1481,11 +1564,8 @@
       <c r="H28" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="J28" s="4" t="n">
-        <v>220</v>
-      </c>
-      <c r="K28" s="0" t="s">
-        <v>131</v>
+      <c r="J28" s="0" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1493,28 +1573,28 @@
         <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="C29" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>134</v>
+        <v>147</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>148</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>14</v>
+        <v>149</v>
       </c>
       <c r="H29" s="0" t="s">
         <v>15</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="K29" s="0" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1522,28 +1602,28 @@
         <v>29</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="C30" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>139</v>
+        <v>153</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>154</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>140</v>
+        <v>155</v>
       </c>
       <c r="H30" s="0" t="s">
         <v>15</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="K30" s="0" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1551,28 +1631,28 @@
         <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="C31" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>145</v>
+        <v>159</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>160</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
       <c r="H31" s="0" t="s">
         <v>15</v>
       </c>
       <c r="J31" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="K31" s="0" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1580,28 +1660,28 @@
         <v>31</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>149</v>
+        <v>163</v>
       </c>
       <c r="C32" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>151</v>
+        <v>164</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>165</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="H32" s="0" t="s">
         <v>15</v>
       </c>
       <c r="J32" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="K32" s="0" t="s">
-        <v>153</v>
+        <v>167</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1609,28 +1689,28 @@
         <v>32</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="C33" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>155</v>
+        <v>169</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>170</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="H33" s="0" t="s">
         <v>15</v>
       </c>
       <c r="J33" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="K33" s="0" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1638,28 +1718,28 @@
         <v>33</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="C34" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>160</v>
+        <v>175</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>176</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="H34" s="0" t="s">
         <v>15</v>
       </c>
       <c r="J34" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="K34" s="0" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1667,28 +1747,28 @@
         <v>34</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
       <c r="C35" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>164</v>
+        <v>54</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>165</v>
+        <v>180</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>181</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>166</v>
+        <v>182</v>
       </c>
       <c r="H35" s="0" t="s">
         <v>15</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="K35" s="0" t="s">
-        <v>168</v>
+        <v>183</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1696,86 +1776,28 @@
         <v>35</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>169</v>
+        <v>184</v>
       </c>
       <c r="C36" s="5" t="n">
         <v>1</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>171</v>
+        <v>185</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>186</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>85</v>
+        <v>187</v>
       </c>
       <c r="H36" s="0" t="s">
         <v>15</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="K36" s="0" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="4" t="n">
-        <v>36</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="C37" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="H37" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J37" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="K37" s="0" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="4" t="n">
-        <v>37</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="C38" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D38" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="E38" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="H38" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J38" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="K38" s="0" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed MCU due to sourcing problems
</commit_message>
<xml_diff>
--- a/icarus_bom.xlsx
+++ b/icarus_bom.xlsx
@@ -547,16 +547,16 @@
     <t xml:space="preserve">U2 </t>
   </si>
   <si>
-    <t xml:space="preserve">STM32G474CEU6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC STM32G474CEU6 48-UFQFPN</t>
+    <t xml:space="preserve">STM32G474CET6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC STM32G474CET6 48-UFQFPN</t>
   </si>
   <si>
     <t xml:space="preserve">48-UFQFPN</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/stmicroelectronics/stm32g474ceu6/10326774</t>
+    <t xml:space="preserve">https://www.digikey.com/en/products/detail/stmicroelectronics/STM32G474CET6/10326773?s=N4IgTCBcDaIMoBUCyBmMBxALAdkwYQFEEA2EAXQF8g</t>
   </si>
   <si>
     <t xml:space="preserve">U3 </t>
@@ -687,7 +687,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -716,6 +716,10 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -735,11 +739,11 @@
   </sheetPr>
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.27"/>
@@ -1697,7 +1701,7 @@
       <c r="D33" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="E33" s="0" t="s">
+      <c r="E33" s="7" t="s">
         <v>169</v>
       </c>
       <c r="F33" s="0" t="s">

</xml_diff>